<commit_message>
had to tweak looking up resources
</commit_message>
<xml_diff>
--- a/RemoveWhatIfScenarios/Default.xlsx
+++ b/RemoveWhatIfScenarios/Default.xlsx
@@ -537,18 +537,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="11.37890625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.1">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -582,7 +582,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
@@ -593,7 +593,7 @@
     <col min="16384" max="16384" width="25.828125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1">
+    <row r="1" customFormat="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>

</xml_diff>